<commit_message>
Filter CytokineExpression on SNP ID
Read the SNPS from the snpsToPlot EMX file and filter the
CytokineExpression entities based on the values in there.
</commit_message>
<xml_diff>
--- a/src/main/resources/cytokine-emx.xlsx
+++ b/src/main/resources/cytokine-emx.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="0" windowWidth="17620" windowHeight="10100" tabRatio="500"/>
+    <workbookView xWindow="7880" yWindow="0" windowWidth="17620" windowHeight="10100" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="2" r:id="rId1"/>
+    <sheet name="Cytokine" sheetId="3" r:id="rId2"/>
+    <sheet name="Stimulus" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -106,6 +108,24 @@
   </si>
   <si>
     <t>aggregateable</t>
+  </si>
+  <si>
+    <t>SnpsToPlot</t>
+  </si>
+  <si>
+    <t>IFNy</t>
+  </si>
+  <si>
+    <t>IL17</t>
+  </si>
+  <si>
+    <t>TNFA</t>
+  </si>
+  <si>
+    <t>E.Coli</t>
+  </si>
+  <si>
+    <t>A.fumigatusconidia</t>
   </si>
 </sst>
 </file>
@@ -512,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -604,8 +624,14 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" t="b">
         <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -769,4 +795,79 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>